<commit_message>
finish first check of the word list
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AVI\PycharmProjects\useGensim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751A583D-86F7-4AED-99DE-4D1041EA13EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21CC8AA-14AD-4E57-8176-EDFD7B3E5E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="1583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1577">
   <si>
     <t>נר"ו</t>
   </si>
@@ -4402,9 +4402,6 @@
     <t>*משמש גם כתואר וגם כחלק ראשון</t>
   </si>
   <si>
-    <t>*יותר מופיע כמקצוע לבד מכתיאור כבוד</t>
-  </si>
-  <si>
     <t>*מופיע גם כשם וגם כתואר</t>
   </si>
   <si>
@@ -4414,42 +4411,21 @@
     <t>*משה ישראל חזן</t>
   </si>
   <si>
-    <t>*לא תואר יותר מקצוע</t>
-  </si>
-  <si>
     <t>*הכונה צבי - לא ברור למה מוסיפים " במילה זו</t>
   </si>
   <si>
-    <t>*מופיע גם כביטוי מורי ואלופי וגם כתואר לתפיק אלופי הקהל וגם כתואר כבוד</t>
-  </si>
-  <si>
     <t>*לא תואר כבוד יותר תיאור - מחבר ספר - כזיהוי</t>
   </si>
   <si>
-    <t xml:space="preserve">*יותר מופיע כמקצוע </t>
-  </si>
-  <si>
     <t>*מציין שנה</t>
   </si>
   <si>
     <t>*חלק מביטוי אור ישראל וקודשו</t>
   </si>
   <si>
-    <t>*כנראה שם פרטי אמצעי בשפה זרה של חכם שמופיע הרבה בטקסט</t>
-  </si>
-  <si>
-    <t>*ידיו ורגליו</t>
-  </si>
-  <si>
-    <t>*מופיע הרבה לא כתואר כבוד לאנשים מסויימים אלא כדיבור על אנשים סתמיים</t>
-  </si>
-  <si>
     <t>*נשמתו בגנזי מרומים</t>
   </si>
   <si>
-    <t>*יותר מקצוע מתואר כבוד</t>
-  </si>
-  <si>
     <t>*להבדיל בין חיים לחיים</t>
   </si>
   <si>
@@ -4459,12 +4435,6 @@
     <t>*לפעמים חלק מתואר אביר הרועים לפעמים תואר אביר יעקב לפעמים ציטוט הפסוק אביר יעקב ולפעמים ספר אביר יעקב</t>
   </si>
   <si>
-    <t>*מופיע בעיקר כדרך לפניה בגוף שלישי ולא כתואר לפני השם</t>
-  </si>
-  <si>
-    <t>*מופיע בעיקר כתפקיד ולא כתואר כבוד</t>
-  </si>
-  <si>
     <t xml:space="preserve">*מופיע הרבה כתואר כבוד אבל גם לא מעט כקיצור למילה "כמות" </t>
   </si>
   <si>
@@ -4492,9 +4462,6 @@
     <t>*הרבה כפניה סתמית</t>
   </si>
   <si>
-    <t>*בעיקר כמקצוע</t>
-  </si>
-  <si>
     <t>*תואר לפני שם של עיר</t>
   </si>
   <si>
@@ -4516,9 +4483,6 @@
     <t>*חלק מביטוי של הרב הראשי של...</t>
   </si>
   <si>
-    <t>*לפעמים מופיע כברכה לאחר הזכרת אנשי מקום כלשהו ולא כתואר לאדם מסויים</t>
-  </si>
-  <si>
     <t>*לפעמים קצת בעייתי - מופיע כחבר של אדם פלוני ולא כתואר כבוד- וכן מופיע כתיאור ל"חבר" במעשרות וישנם איזכורים לחבר בספר הכוזרי אך ישנם גם לא מעט הופעות כתואר כבוד לרב</t>
   </si>
   <si>
@@ -4528,9 +4492,6 @@
     <t>*הרבה פעים כחלק מביטוי "סבא דמשפטים" שבא כתואר כבוד</t>
   </si>
   <si>
-    <t>*יותר תפקיד מתואר כבוד</t>
-  </si>
-  <si>
     <t>*כנראהתואר כבוד לא הבנתי מה הפתיחה</t>
   </si>
   <si>
@@ -4579,9 +4540,6 @@
     <t>*יותר מוסיע ביחס לספרים וכתבים, וכן ישנו ספר הבהיר , וכן ישנם מקומות שהכוונה שהוא הבהיר את דבריו</t>
   </si>
   <si>
-    <t>*תואר ענווה עצמי זה תואר כבוד?</t>
-  </si>
-  <si>
     <t>*לא כבוד בדויק, מחבר ספר זה ציון לצורך זיהוי</t>
   </si>
   <si>
@@ -4597,12 +4555,6 @@
     <t>*גברא רבה ויקירא אך מופיע גם ביחס לדברים נוספים כגון מחילה רבה ויקירא או ב"ד רבה ויקירא</t>
   </si>
   <si>
-    <t>*כבוד אך גם מקצוע</t>
-  </si>
-  <si>
-    <t>*ככל הנראה דקהילת או משהו בסיגנון</t>
-  </si>
-  <si>
     <t>*ישנם גם אזכורים שאינם קשורים לכבוד כגון בית הדין הרבני</t>
   </si>
   <si>
@@ -4621,36 +4573,21 @@
     <t>*מחתם סופר, מחרם סתם, וגם מחבר ספר זה לא כל כך תואר כבוד אלא ציון לצורך זיהוי</t>
   </si>
   <si>
-    <t>*תפקיד יותר מכבוד</t>
-  </si>
-  <si>
     <t xml:space="preserve">* כנראה יראה זרע יאריך ימים אמן </t>
   </si>
   <si>
     <t>*כנל לגבי שאר המוצים</t>
   </si>
   <si>
-    <t xml:space="preserve">*אולי זה הפוך מתואר כבוד? </t>
-  </si>
-  <si>
     <t>*לא רק במובן הצבאי אלא גם תואר לחשיבות ושררה</t>
   </si>
   <si>
-    <t>*כנל לגבי אבד</t>
-  </si>
-  <si>
     <t>* יכוננה בצדק - זה תיאור למקומות ולא לאנשים</t>
   </si>
   <si>
-    <t>*הרבה פעמים מופיע כשער הזקן או לאדם שהוא הזדקן וקיים מספר מסויים של תארים של זקן (הרבה גם מתוך כינויי הראשונים והתנאים: שמאי הזקן ר"י הזקן)</t>
-  </si>
-  <si>
     <t>*אחר דרישת שלומו הטוב</t>
   </si>
   <si>
-    <t>*כנל לגבי אב"ד</t>
-  </si>
-  <si>
     <t>*לפעמים מציין סימן</t>
   </si>
   <si>
@@ -4681,9 +4618,6 @@
     <t>*הדיין המצוין</t>
   </si>
   <si>
-    <t>*כנל לגבי ראבד</t>
-  </si>
-  <si>
     <t>*מופעי ככבוד אך גם כתאור לאדם סתמי שהוא אברך וכן כעתיד גוף ראשון של ברך - אני אברך אותך</t>
   </si>
   <si>
@@ -4696,9 +4630,6 @@
     <t>*רום פאר מעלתו</t>
   </si>
   <si>
-    <t>*כנל לגבי מוץ</t>
-  </si>
-  <si>
     <t>*מופיע גם כתואר כבוד אך גם הרבה כחלק משם של ספר</t>
   </si>
   <si>
@@ -4738,9 +4669,6 @@
     <t>*קצת מסופק לגבי זה, מופיע בעיקר כ נתכבדתי ביקרתו</t>
   </si>
   <si>
-    <t>*למעלה - הנזכר למעלה</t>
-  </si>
-  <si>
     <t>*בוצינא דנהורא</t>
   </si>
   <si>
@@ -4768,7 +4696,61 @@
     <t>*מופיע גם ביחס לדברים</t>
   </si>
   <si>
-    <t>*האבה פעמים מופיע בהקשרים שונים לא קשורים, כנראה גם ראשי תיבות של חכם או ספר</t>
+    <t>*זה מופיע כתיאור עצמי ולא כתואר לאחרים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*בהתחלה חשבתי שזה יותר מופיע כמקצוע לבד מכתיאור כבוד אך החלטתי שזה כן עונה להגדרה </t>
+  </si>
+  <si>
+    <t>*בהתחלה חשבתי שזה לא תואר אלא יותר מקצוע אך החלטתי שעונה להגדרה</t>
+  </si>
+  <si>
+    <t>*כנ"ל לגבי המו"ץ</t>
+  </si>
+  <si>
+    <t>*מופיע גם כביטוי מורי ואלופי וגם כתואר לתפקיד אלופי הקהל וגם כתואר כבוד</t>
+  </si>
+  <si>
+    <t>*כנל לגבי מו"ץ</t>
+  </si>
+  <si>
+    <t>*מופיע כידיו ורגליו אך גם כיורנו רבנו וכיושב ראש</t>
+  </si>
+  <si>
+    <t>*מופיע הרבה לא כתואר כבוד לאנשים מסויימים אלא כדיבור על אנשים סתמיים אך עדיין זה תואר</t>
+  </si>
+  <si>
+    <t>*כנ"ל לגבי מו"ץ</t>
+  </si>
+  <si>
+    <t>*מופיע בעיקר כדרך לפניה בגוף שלישי ולא כתואר לפני השם אך זו עדיין פניה של תואר כבוד</t>
+  </si>
+  <si>
+    <t>*לפעמים מופיע כברכה לאחר הזכרת אנשי מקום כלשהו ולא ביחס לאדם מסויים</t>
+  </si>
+  <si>
+    <t>*תואר עצמי לא לאחרים</t>
+  </si>
+  <si>
+    <t>*ככל הנראה דקהילת</t>
+  </si>
+  <si>
+    <t>*הרבה פעמים מופיע כשיער הזקן או לאדם שהוא הזדקן וקיים מספר מסויים של תארים של זקן (הרבה גם מתוך כינויי הראשונים והתנאים: שמאי הזקן ר"י הזקן)</t>
+  </si>
+  <si>
+    <t>*כנ" לגבי מו"ץ</t>
+  </si>
+  <si>
+    <t>*מופיע כראיה וכחלק מתואר מופת הדור</t>
+  </si>
+  <si>
+    <t>*למעלה - הנזכר למעלה וכן כתואר כבוד</t>
+  </si>
+  <si>
+    <t>*הרבה פעמים מופיע בהקשרים שונים לא קשורים, כנראה גם ראשי תיבות של חכם או ספר</t>
+  </si>
+  <si>
+    <t>*בהתחלה חשבתי להוציא את זה כי זה מופיע גם כמקצוע, אך החלטתי שבהרבה הקשרים זה כן עונה להגדרה</t>
   </si>
 </sst>
 </file>
@@ -5144,20 +5126,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1454"/>
+  <dimension ref="A1:I1454"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1452" sqref="C1452"/>
+      <selection activeCell="M189" sqref="M189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I1" t="s">
         <v>1453</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5168,7 +5150,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5179,7 +5161,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5190,7 +5172,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5198,7 +5180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5206,7 +5188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5214,7 +5196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5222,7 +5204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5230,81 +5212,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="M10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="M11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="M12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="M13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="M14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="M15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -5563,7 +5524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -5571,18 +5532,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
-      <c r="J50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -5590,7 +5548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -5598,7 +5556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -5606,7 +5564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -5614,7 +5572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -5622,7 +5580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -5630,7 +5588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -5638,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -5646,7 +5604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -5654,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -5662,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -5670,7 +5628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -5678,7 +5636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -5686,7 +5644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -6337,7 +6295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -6345,7 +6303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -6353,29 +6311,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
       <c r="B147">
         <v>1</v>
       </c>
-      <c r="I147" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
       <c r="B148">
         <v>4</v>
       </c>
-      <c r="H148" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -6383,7 +6335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -6391,7 +6343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -6399,7 +6351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -6407,7 +6359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -6415,7 +6367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>152</v>
       </c>
@@ -6423,7 +6375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -6431,7 +6383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -6439,7 +6391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -6447,7 +6399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -6455,7 +6407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -6463,7 +6415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -6733,7 +6685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -6741,7 +6693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -6749,7 +6701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>193</v>
       </c>
@@ -6757,7 +6709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>194</v>
       </c>
@@ -6765,7 +6717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>195</v>
       </c>
@@ -6773,7 +6725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>196</v>
       </c>
@@ -6781,7 +6733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>197</v>
       </c>
@@ -6789,18 +6741,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>198</v>
       </c>
       <c r="B200">
         <v>1</v>
       </c>
-      <c r="J200" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -6808,7 +6757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>200</v>
       </c>
@@ -6816,7 +6765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>201</v>
       </c>
@@ -6824,7 +6773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>202</v>
       </c>
@@ -6832,7 +6781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>203</v>
       </c>
@@ -6840,7 +6789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>204</v>
       </c>
@@ -6848,7 +6797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>205</v>
       </c>
@@ -6856,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>206</v>
       </c>
@@ -6869,10 +6818,10 @@
         <v>207</v>
       </c>
       <c r="B209">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C209" t="s">
-        <v>1460</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -6939,7 +6888,7 @@
         <v>4</v>
       </c>
       <c r="C217" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
@@ -7054,7 +7003,7 @@
         <v>1</v>
       </c>
       <c r="C231" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
@@ -7088,6 +7037,9 @@
       <c r="B235">
         <v>2</v>
       </c>
+      <c r="C235" t="s">
+        <v>1558</v>
+      </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
@@ -7169,7 +7121,7 @@
         <v>2</v>
       </c>
       <c r="C245" t="s">
-        <v>1460</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
@@ -7193,7 +7145,7 @@
         <v>246</v>
       </c>
       <c r="B248">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -7436,7 +7388,7 @@
         <v>4</v>
       </c>
       <c r="C278" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -7444,10 +7396,10 @@
         <v>277</v>
       </c>
       <c r="B279">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C279" t="s">
-        <v>1464</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
@@ -7498,7 +7450,7 @@
         <v>4</v>
       </c>
       <c r="C285" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
@@ -7653,29 +7605,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>303</v>
       </c>
       <c r="B305">
         <v>1</v>
       </c>
-      <c r="J305" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>304</v>
       </c>
       <c r="B306">
         <v>2</v>
       </c>
-      <c r="J306" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>305</v>
       </c>
@@ -7683,18 +7629,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>306</v>
       </c>
       <c r="B308">
         <v>4</v>
       </c>
-      <c r="J308" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>307</v>
       </c>
@@ -7702,7 +7645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>308</v>
       </c>
@@ -7710,7 +7653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>309</v>
       </c>
@@ -7718,7 +7661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>310</v>
       </c>
@@ -7726,7 +7669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>311</v>
       </c>
@@ -7734,7 +7677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>312</v>
       </c>
@@ -7742,18 +7685,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>313</v>
       </c>
       <c r="B315">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C315" t="s">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>314</v>
       </c>
@@ -7761,7 +7704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>315</v>
       </c>
@@ -7769,7 +7712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>316</v>
       </c>
@@ -7777,7 +7720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>317</v>
       </c>
@@ -7785,7 +7728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>318</v>
       </c>
@@ -7921,18 +7864,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>335</v>
       </c>
       <c r="B337">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C337" t="s">
-        <v>1466</v>
-      </c>
-    </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>336</v>
       </c>
@@ -7940,7 +7883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>337</v>
       </c>
@@ -7948,7 +7891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>338</v>
       </c>
@@ -7956,7 +7899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>339</v>
       </c>
@@ -7964,7 +7907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>340</v>
       </c>
@@ -7972,7 +7915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>341</v>
       </c>
@@ -7980,7 +7923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>342</v>
       </c>
@@ -7988,7 +7931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>343</v>
       </c>
@@ -7996,7 +7939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>344</v>
       </c>
@@ -8004,10 +7947,10 @@
         <v>3</v>
       </c>
       <c r="C346" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>345</v>
       </c>
@@ -8015,7 +7958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>346</v>
       </c>
@@ -8023,7 +7966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>347</v>
       </c>
@@ -8031,7 +7974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>348</v>
       </c>
@@ -8039,7 +7982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>349</v>
       </c>
@@ -8047,15 +7990,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>350</v>
       </c>
       <c r="B352">
         <v>2</v>
-      </c>
-      <c r="J352" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
@@ -8415,10 +8355,10 @@
         <v>395</v>
       </c>
       <c r="B397">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C397" t="s">
-        <v>1468</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
@@ -8573,7 +8513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>415</v>
       </c>
@@ -8581,7 +8521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>416</v>
       </c>
@@ -8589,7 +8529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>417</v>
       </c>
@@ -8597,7 +8537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>418</v>
       </c>
@@ -8605,7 +8545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>419</v>
       </c>
@@ -8613,7 +8553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>420</v>
       </c>
@@ -8621,7 +8561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>421</v>
       </c>
@@ -8629,7 +8569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>422</v>
       </c>
@@ -8637,7 +8577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>423</v>
       </c>
@@ -8645,7 +8585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>424</v>
       </c>
@@ -8653,7 +8593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>425</v>
       </c>
@@ -8661,7 +8601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>426</v>
       </c>
@@ -8669,13 +8609,10 @@
         <v>2</v>
       </c>
       <c r="C428" t="s">
-        <v>1469</v>
-      </c>
-      <c r="J428" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>427</v>
       </c>
@@ -8683,7 +8620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>428</v>
       </c>
@@ -8691,7 +8628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>429</v>
       </c>
@@ -8699,7 +8636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>430</v>
       </c>
@@ -8811,7 +8748,7 @@
         <v>1</v>
       </c>
       <c r="C445" t="s">
-        <v>1470</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.2">
@@ -9035,10 +8972,7 @@
         <v>471</v>
       </c>
       <c r="B473">
-        <v>2</v>
-      </c>
-      <c r="C473" t="s">
-        <v>1471</v>
+        <v>1</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.2">
@@ -9046,10 +8980,10 @@
         <v>472</v>
       </c>
       <c r="B474">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C474" t="s">
-        <v>1472</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.2">
@@ -9100,7 +9034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="481" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>479</v>
       </c>
@@ -9108,7 +9042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="482" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>480</v>
       </c>
@@ -9116,7 +9050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="483" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>481</v>
       </c>
@@ -9124,7 +9058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>482</v>
       </c>
@@ -9132,18 +9066,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="485" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>483</v>
       </c>
       <c r="B485">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C485" t="s">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="486" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>484</v>
       </c>
@@ -9151,7 +9085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="487" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>485</v>
       </c>
@@ -9159,7 +9093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="488" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>486</v>
       </c>
@@ -9167,7 +9101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="489" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>487</v>
       </c>
@@ -9175,7 +9109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="490" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>488</v>
       </c>
@@ -9183,7 +9117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="491" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>489</v>
       </c>
@@ -9191,7 +9125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>490</v>
       </c>
@@ -9199,7 +9133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="493" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>491</v>
       </c>
@@ -9207,7 +9141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="494" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>492</v>
       </c>
@@ -9215,18 +9149,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="495" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>493</v>
       </c>
       <c r="B495">
         <v>2</v>
       </c>
-      <c r="J495" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>494</v>
       </c>
@@ -9546,7 +9477,7 @@
         <v>1</v>
       </c>
       <c r="C535" t="s">
-        <v>1474</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.2">
@@ -9594,10 +9525,10 @@
         <v>539</v>
       </c>
       <c r="B541">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C541" t="s">
-        <v>1475</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.2">
@@ -9656,7 +9587,7 @@
         <v>2</v>
       </c>
       <c r="C548" t="s">
-        <v>1476</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.2">
@@ -9755,7 +9686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="561" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>559</v>
       </c>
@@ -9763,7 +9694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="562" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>560</v>
       </c>
@@ -9771,7 +9702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="563" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>561</v>
       </c>
@@ -9779,7 +9710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="564" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>562</v>
       </c>
@@ -9787,7 +9718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="565" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>563</v>
       </c>
@@ -9795,7 +9726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="566" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>564</v>
       </c>
@@ -9803,40 +9734,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="567" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>565</v>
       </c>
       <c r="B567">
         <v>2</v>
       </c>
-      <c r="J567" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="568" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>566</v>
       </c>
       <c r="B568">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C568" t="s">
-        <v>1477</v>
-      </c>
-    </row>
-    <row r="569" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>567</v>
       </c>
       <c r="B569">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C569" t="s">
-        <v>1478</v>
-      </c>
-    </row>
-    <row r="570" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>568</v>
       </c>
@@ -9844,7 +9772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="571" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>569</v>
       </c>
@@ -9852,7 +9780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="572" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
         <v>570</v>
       </c>
@@ -9860,7 +9788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="573" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
         <v>571</v>
       </c>
@@ -9868,7 +9796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="574" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>572</v>
       </c>
@@ -9876,7 +9804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="575" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
         <v>573</v>
       </c>
@@ -9884,7 +9812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="576" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
         <v>574</v>
       </c>
@@ -9905,10 +9833,10 @@
         <v>576</v>
       </c>
       <c r="B578">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C578" t="s">
-        <v>1479</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.2">
@@ -9924,10 +9852,10 @@
         <v>578</v>
       </c>
       <c r="B580">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C580" t="s">
-        <v>1480</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.2">
@@ -9935,10 +9863,10 @@
         <v>579</v>
       </c>
       <c r="B581">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C581" t="s">
-        <v>1481</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.2">
@@ -10106,10 +10034,10 @@
         <v>600</v>
       </c>
       <c r="B602">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C602" t="s">
-        <v>1482</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.2">
@@ -10232,7 +10160,7 @@
         <v>2</v>
       </c>
       <c r="C617" t="s">
-        <v>1483</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.2">
@@ -10283,7 +10211,7 @@
         <v>2</v>
       </c>
       <c r="C623" t="s">
-        <v>1484</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.2">
@@ -10355,10 +10283,10 @@
         <v>630</v>
       </c>
       <c r="B632">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C632" t="s">
-        <v>1475</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.2">
@@ -10369,7 +10297,7 @@
         <v>1</v>
       </c>
       <c r="C633" t="s">
-        <v>1485</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.2">
@@ -10465,10 +10393,10 @@
         <v>643</v>
       </c>
       <c r="B645">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C645" t="s">
-        <v>1486</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.2">
@@ -10535,7 +10463,7 @@
         <v>2</v>
       </c>
       <c r="C653" t="s">
-        <v>1487</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.2">
@@ -10554,7 +10482,7 @@
         <v>2</v>
       </c>
       <c r="C655" t="s">
-        <v>1488</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.2">
@@ -10581,7 +10509,7 @@
         <v>1</v>
       </c>
       <c r="C658" t="s">
-        <v>1489</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.2">
@@ -10605,10 +10533,10 @@
         <v>659</v>
       </c>
       <c r="B661">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C661" t="s">
-        <v>1490</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.2">
@@ -10675,7 +10603,7 @@
         <v>2</v>
       </c>
       <c r="C669" t="s">
-        <v>1491</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.2">
@@ -10755,10 +10683,10 @@
         <v>677</v>
       </c>
       <c r="B679">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C679" t="s">
-        <v>1475</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="680" spans="1:3" x14ac:dyDescent="0.2">
@@ -10862,10 +10790,10 @@
         <v>690</v>
       </c>
       <c r="B692">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C692" t="s">
-        <v>1475</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="693" spans="1:3" x14ac:dyDescent="0.2">
@@ -10892,7 +10820,7 @@
         <v>2</v>
       </c>
       <c r="C695" t="s">
-        <v>1492</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="696" spans="1:3" x14ac:dyDescent="0.2">
@@ -10991,7 +10919,7 @@
         <v>1</v>
       </c>
       <c r="C707" t="s">
-        <v>1493</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="708" spans="1:3" x14ac:dyDescent="0.2">
@@ -11047,7 +10975,7 @@
         <v>712</v>
       </c>
       <c r="B714">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.2">
@@ -11066,7 +10994,7 @@
         <v>1</v>
       </c>
       <c r="C716" t="s">
-        <v>1494</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.2">
@@ -11149,7 +11077,7 @@
         <v>1</v>
       </c>
       <c r="C726" t="s">
-        <v>1495</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="727" spans="1:3" x14ac:dyDescent="0.2">
@@ -11192,7 +11120,7 @@
         <v>1</v>
       </c>
       <c r="C731" t="s">
-        <v>1496</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="732" spans="1:3" x14ac:dyDescent="0.2">
@@ -11208,10 +11136,10 @@
         <v>731</v>
       </c>
       <c r="B733">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C733" t="s">
-        <v>1497</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.2">
@@ -11278,7 +11206,7 @@
         <v>1</v>
       </c>
       <c r="C741" t="s">
-        <v>1498</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.2">
@@ -11305,7 +11233,7 @@
         <v>1</v>
       </c>
       <c r="C744" t="s">
-        <v>1499</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.2">
@@ -11316,7 +11244,7 @@
         <v>2</v>
       </c>
       <c r="C745" t="s">
-        <v>1500</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="746" spans="1:3" x14ac:dyDescent="0.2">
@@ -11324,10 +11252,10 @@
         <v>744</v>
       </c>
       <c r="B746">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C746" t="s">
-        <v>1501</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.2">
@@ -11495,10 +11423,10 @@
         <v>765</v>
       </c>
       <c r="B767">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C767" t="s">
-        <v>1502</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.2">
@@ -11549,7 +11477,7 @@
         <v>1</v>
       </c>
       <c r="C773" t="s">
-        <v>1503</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.2">
@@ -11576,7 +11504,7 @@
         <v>1</v>
       </c>
       <c r="C776" t="s">
-        <v>1504</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.2">
@@ -11627,7 +11555,7 @@
         <v>1</v>
       </c>
       <c r="C782" t="s">
-        <v>1505</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="783" spans="1:3" x14ac:dyDescent="0.2">
@@ -11694,7 +11622,7 @@
         <v>1</v>
       </c>
       <c r="C790" t="s">
-        <v>1506</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.2">
@@ -11705,7 +11633,7 @@
         <v>3</v>
       </c>
       <c r="C791" t="s">
-        <v>1507</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.2">
@@ -11737,10 +11665,10 @@
         <v>793</v>
       </c>
       <c r="B795">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C795" t="s">
-        <v>793</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="796" spans="1:3" x14ac:dyDescent="0.2">
@@ -11750,9 +11678,6 @@
       <c r="B796">
         <v>2</v>
       </c>
-      <c r="C796" t="s">
-        <v>1475</v>
-      </c>
     </row>
     <row r="797" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A797" t="s">
@@ -11762,7 +11687,7 @@
         <v>3</v>
       </c>
       <c r="C797" t="s">
-        <v>1508</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="798" spans="1:3" x14ac:dyDescent="0.2">
@@ -11837,7 +11762,7 @@
         <v>4</v>
       </c>
       <c r="C806" t="s">
-        <v>1509</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.2">
@@ -11896,7 +11821,7 @@
         <v>1</v>
       </c>
       <c r="C813" t="s">
-        <v>1510</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.2">
@@ -11955,7 +11880,7 @@
         <v>2</v>
       </c>
       <c r="C820" t="s">
-        <v>1511</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.2">
@@ -12038,7 +11963,7 @@
         <v>1</v>
       </c>
       <c r="C830" t="s">
-        <v>1512</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.2">
@@ -12054,10 +11979,10 @@
         <v>830</v>
       </c>
       <c r="B832">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C832" t="s">
-        <v>1513</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.2">
@@ -12100,7 +12025,7 @@
         <v>1</v>
       </c>
       <c r="C837" t="s">
-        <v>1514</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.2">
@@ -12143,7 +12068,7 @@
         <v>1</v>
       </c>
       <c r="C842" t="s">
-        <v>1515</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="843" spans="1:3" x14ac:dyDescent="0.2">
@@ -12170,7 +12095,7 @@
         <v>1</v>
       </c>
       <c r="C845" t="s">
-        <v>1516</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.2">
@@ -12229,7 +12154,7 @@
         <v>3</v>
       </c>
       <c r="C852" t="s">
-        <v>1517</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.2">
@@ -12320,7 +12245,7 @@
         <v>2</v>
       </c>
       <c r="C863" t="s">
-        <v>1518</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.2">
@@ -12336,10 +12261,10 @@
         <v>863</v>
       </c>
       <c r="B865">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C865" t="s">
-        <v>1519</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.2">
@@ -12406,7 +12331,7 @@
         <v>3</v>
       </c>
       <c r="C873" t="s">
-        <v>1520</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.2">
@@ -12441,7 +12366,7 @@
         <v>3</v>
       </c>
       <c r="C877" t="s">
-        <v>1521</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.2">
@@ -12548,7 +12473,7 @@
         <v>1</v>
       </c>
       <c r="C890" t="s">
-        <v>1522</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.2">
@@ -12647,7 +12572,7 @@
         <v>1</v>
       </c>
       <c r="C902" t="s">
-        <v>1523</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.2">
@@ -12786,7 +12711,7 @@
         <v>1</v>
       </c>
       <c r="C919" t="s">
-        <v>1524</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="920" spans="1:3" x14ac:dyDescent="0.2">
@@ -12829,7 +12754,7 @@
         <v>1</v>
       </c>
       <c r="C924" t="s">
-        <v>1525</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="925" spans="1:3" x14ac:dyDescent="0.2">
@@ -12848,7 +12773,7 @@
         <v>2</v>
       </c>
       <c r="C926" t="s">
-        <v>1526</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="927" spans="1:3" x14ac:dyDescent="0.2">
@@ -12872,7 +12797,7 @@
         <v>927</v>
       </c>
       <c r="B929">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="930" spans="1:3" x14ac:dyDescent="0.2">
@@ -12907,7 +12832,7 @@
         <v>1</v>
       </c>
       <c r="C933" t="s">
-        <v>1527</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.2">
@@ -12918,7 +12843,7 @@
         <v>3</v>
       </c>
       <c r="C934" t="s">
-        <v>1528</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.2">
@@ -12993,7 +12918,7 @@
         <v>2</v>
       </c>
       <c r="C943" t="s">
-        <v>1529</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.2">
@@ -13012,7 +12937,7 @@
         <v>1</v>
       </c>
       <c r="C945" t="s">
-        <v>1530</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.2">
@@ -13063,7 +12988,7 @@
         <v>4</v>
       </c>
       <c r="C951" t="s">
-        <v>1531</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="952" spans="1:3" x14ac:dyDescent="0.2">
@@ -13074,7 +12999,7 @@
         <v>2</v>
       </c>
       <c r="C952" t="s">
-        <v>1532</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="953" spans="1:3" x14ac:dyDescent="0.2">
@@ -13178,10 +13103,10 @@
         <v>963</v>
       </c>
       <c r="B965">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C965" t="s">
-        <v>1533</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="966" spans="1:3" x14ac:dyDescent="0.2">
@@ -13197,10 +13122,10 @@
         <v>965</v>
       </c>
       <c r="B967">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C967" t="s">
-        <v>1534</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="968" spans="1:3" x14ac:dyDescent="0.2">
@@ -13208,10 +13133,10 @@
         <v>966</v>
       </c>
       <c r="B968">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C968" t="s">
-        <v>1535</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="969" spans="1:3" x14ac:dyDescent="0.2">
@@ -13307,10 +13232,10 @@
         <v>978</v>
       </c>
       <c r="B980">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C980" t="s">
-        <v>1536</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="981" spans="1:3" x14ac:dyDescent="0.2">
@@ -13393,7 +13318,7 @@
         <v>1</v>
       </c>
       <c r="C990" t="s">
-        <v>1537</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="991" spans="1:3" x14ac:dyDescent="0.2">
@@ -13433,10 +13358,10 @@
         <v>993</v>
       </c>
       <c r="B995">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C995" t="s">
-        <v>1538</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="996" spans="1:3" x14ac:dyDescent="0.2">
@@ -13511,7 +13436,7 @@
         <v>2</v>
       </c>
       <c r="C1004" t="s">
-        <v>1539</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1005" spans="1:3" x14ac:dyDescent="0.2">
@@ -13642,7 +13567,7 @@
         <v>2</v>
       </c>
       <c r="C1020" t="s">
-        <v>1540</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="1021" spans="1:3" x14ac:dyDescent="0.2">
@@ -13677,7 +13602,7 @@
         <v>2</v>
       </c>
       <c r="C1024" t="s">
-        <v>1541</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1025" spans="1:3" x14ac:dyDescent="0.2">
@@ -13717,10 +13642,10 @@
         <v>1027</v>
       </c>
       <c r="B1029">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1029" t="s">
-        <v>1542</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="1030" spans="1:3" x14ac:dyDescent="0.2">
@@ -13739,7 +13664,7 @@
         <v>4</v>
       </c>
       <c r="C1031" t="s">
-        <v>1543</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1032" spans="1:3" x14ac:dyDescent="0.2">
@@ -13750,7 +13675,7 @@
         <v>3</v>
       </c>
       <c r="C1032" t="s">
-        <v>1544</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1033" spans="1:3" x14ac:dyDescent="0.2">
@@ -13825,7 +13750,7 @@
         <v>1</v>
       </c>
       <c r="C1041" t="s">
-        <v>1545</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1042" spans="1:3" x14ac:dyDescent="0.2">
@@ -13860,7 +13785,7 @@
         <v>2</v>
       </c>
       <c r="C1045" t="s">
-        <v>1546</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1046" spans="1:3" x14ac:dyDescent="0.2">
@@ -13903,7 +13828,7 @@
         <v>2</v>
       </c>
       <c r="C1050" t="s">
-        <v>1547</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1051" spans="1:3" x14ac:dyDescent="0.2">
@@ -13978,7 +13903,7 @@
         <v>1</v>
       </c>
       <c r="C1059" t="s">
-        <v>1548</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1060" spans="1:3" x14ac:dyDescent="0.2">
@@ -14157,7 +14082,7 @@
         <v>2</v>
       </c>
       <c r="C1081" t="s">
-        <v>1549</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1082" spans="1:3" x14ac:dyDescent="0.2">
@@ -14216,7 +14141,7 @@
         <v>1</v>
       </c>
       <c r="C1088" t="s">
-        <v>1550</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1089" spans="1:3" x14ac:dyDescent="0.2">
@@ -14243,7 +14168,7 @@
         <v>1</v>
       </c>
       <c r="C1091" t="s">
-        <v>1551</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1092" spans="1:3" x14ac:dyDescent="0.2">
@@ -14286,7 +14211,7 @@
         <v>1</v>
       </c>
       <c r="C1096" t="s">
-        <v>1552</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1097" spans="1:3" x14ac:dyDescent="0.2">
@@ -14329,7 +14254,7 @@
         <v>1</v>
       </c>
       <c r="C1101" t="s">
-        <v>1553</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1102" spans="1:3" x14ac:dyDescent="0.2">
@@ -14340,7 +14265,7 @@
         <v>3</v>
       </c>
       <c r="C1102" t="s">
-        <v>1554</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1103" spans="1:3" x14ac:dyDescent="0.2">
@@ -14375,7 +14300,7 @@
         <v>2</v>
       </c>
       <c r="C1106" t="s">
-        <v>1555</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1107" spans="1:3" x14ac:dyDescent="0.2">
@@ -14410,7 +14335,7 @@
         <v>1</v>
       </c>
       <c r="C1110" t="s">
-        <v>1556</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1111" spans="1:3" x14ac:dyDescent="0.2">
@@ -14509,7 +14434,7 @@
         <v>1</v>
       </c>
       <c r="C1122" t="s">
-        <v>1557</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1123" spans="1:3" x14ac:dyDescent="0.2">
@@ -14621,10 +14546,10 @@
         <v>1134</v>
       </c>
       <c r="B1136">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1136" t="s">
-        <v>1558</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
@@ -14835,7 +14760,7 @@
         <v>3</v>
       </c>
       <c r="C1162" t="s">
-        <v>1559</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1163" spans="1:3" x14ac:dyDescent="0.2">
@@ -14846,7 +14771,7 @@
         <v>1</v>
       </c>
       <c r="C1163" t="s">
-        <v>1560</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1164" spans="1:3" x14ac:dyDescent="0.2">
@@ -14929,7 +14854,7 @@
         <v>1</v>
       </c>
       <c r="C1173" t="s">
-        <v>1477</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1174" spans="1:3" x14ac:dyDescent="0.2">
@@ -15028,7 +14953,7 @@
         <v>2</v>
       </c>
       <c r="C1185" t="s">
-        <v>1561</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1186" spans="1:3" x14ac:dyDescent="0.2">
@@ -15143,7 +15068,7 @@
         <v>1</v>
       </c>
       <c r="C1199" t="s">
-        <v>1562</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1200" spans="1:3" x14ac:dyDescent="0.2">
@@ -15151,10 +15076,10 @@
         <v>1198</v>
       </c>
       <c r="B1200">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1200" t="s">
-        <v>1538</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1201" spans="1:3" x14ac:dyDescent="0.2">
@@ -15170,10 +15095,10 @@
         <v>1200</v>
       </c>
       <c r="B1202">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1202" t="s">
-        <v>1538</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1203" spans="1:3" x14ac:dyDescent="0.2">
@@ -15184,7 +15109,7 @@
         <v>2</v>
       </c>
       <c r="C1203" t="s">
-        <v>1563</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1204" spans="1:3" x14ac:dyDescent="0.2">
@@ -15211,7 +15136,7 @@
         <v>1</v>
       </c>
       <c r="C1206" t="s">
-        <v>1564</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1207" spans="1:3" x14ac:dyDescent="0.2">
@@ -15238,7 +15163,7 @@
         <v>1</v>
       </c>
       <c r="C1209" t="s">
-        <v>1565</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1210" spans="1:3" x14ac:dyDescent="0.2">
@@ -15265,7 +15190,7 @@
         <v>3</v>
       </c>
       <c r="C1212" t="s">
-        <v>1566</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="1213" spans="1:3" x14ac:dyDescent="0.2">
@@ -15316,7 +15241,7 @@
         <v>2</v>
       </c>
       <c r="C1218" t="s">
-        <v>1567</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="1219" spans="1:3" x14ac:dyDescent="0.2">
@@ -15383,7 +15308,7 @@
         <v>2</v>
       </c>
       <c r="C1226" t="s">
-        <v>1568</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="1227" spans="1:3" x14ac:dyDescent="0.2">
@@ -15391,10 +15316,10 @@
         <v>1225</v>
       </c>
       <c r="B1227">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1227" t="s">
-        <v>1558</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1228" spans="1:3" x14ac:dyDescent="0.2">
@@ -15410,7 +15335,10 @@
         <v>1227</v>
       </c>
       <c r="B1229">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>1573</v>
       </c>
     </row>
     <row r="1230" spans="1:3" x14ac:dyDescent="0.2">
@@ -15421,7 +15349,7 @@
         <v>1</v>
       </c>
       <c r="C1230" t="s">
-        <v>1569</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="1231" spans="1:3" x14ac:dyDescent="0.2">
@@ -15888,7 +15816,7 @@
         <v>1</v>
       </c>
       <c r="C1288" t="s">
-        <v>1570</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1289" spans="1:3" x14ac:dyDescent="0.2">
@@ -16259,7 +16187,7 @@
         <v>1</v>
       </c>
       <c r="C1334" t="s">
-        <v>1571</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1335" spans="1:3" x14ac:dyDescent="0.2">
@@ -16483,10 +16411,10 @@
         <v>1360</v>
       </c>
       <c r="B1362">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1362" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1363" spans="1:3" x14ac:dyDescent="0.2">
@@ -16513,7 +16441,7 @@
         <v>1</v>
       </c>
       <c r="C1365" t="s">
-        <v>1573</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="1366" spans="1:3" x14ac:dyDescent="0.2">
@@ -16532,7 +16460,7 @@
         <v>1</v>
       </c>
       <c r="C1367" t="s">
-        <v>1574</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="1368" spans="1:3" x14ac:dyDescent="0.2">
@@ -16591,7 +16519,7 @@
         <v>1</v>
       </c>
       <c r="C1374" t="s">
-        <v>1575</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1375" spans="1:3" x14ac:dyDescent="0.2">
@@ -16618,7 +16546,7 @@
         <v>1</v>
       </c>
       <c r="C1377" t="s">
-        <v>1576</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1378" spans="1:3" x14ac:dyDescent="0.2">
@@ -16773,7 +16701,7 @@
         <v>4</v>
       </c>
       <c r="C1396" t="s">
-        <v>1577</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="1397" spans="1:3" x14ac:dyDescent="0.2">
@@ -16824,7 +16752,7 @@
         <v>1</v>
       </c>
       <c r="C1402" t="s">
-        <v>1578</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="1403" spans="1:3" x14ac:dyDescent="0.2">
@@ -16867,7 +16795,7 @@
         <v>1</v>
       </c>
       <c r="C1407" t="s">
-        <v>1579</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="1408" spans="1:3" x14ac:dyDescent="0.2">
@@ -16974,7 +16902,7 @@
         <v>1</v>
       </c>
       <c r="C1420" t="s">
-        <v>1580</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="1421" spans="1:3" x14ac:dyDescent="0.2">
@@ -17169,7 +17097,7 @@
         <v>1</v>
       </c>
       <c r="C1444" t="s">
-        <v>1581</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="1445" spans="1:3" x14ac:dyDescent="0.2">
@@ -17228,7 +17156,7 @@
         <v>2</v>
       </c>
       <c r="C1451" t="s">
-        <v>1582</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="1452" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>